<commit_message>
Entropy Sketch Low Dimensions Experiments
</commit_message>
<xml_diff>
--- a/Experiments/Inner Product/Inner Product Dimension/combined.xlsx
+++ b/Experiments/Inner Product/Inner Product Dimension/combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuval\Desktop\Distributed Monitoring Thesis\Experiments\Inner Product\Inner Product Dimension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34F5F9B-D9A6-41E0-A33F-A1B49704A7E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802265CF-393E-436B-AF6C-613D44247206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1290,6 +1290,37 @@
           <c:yVal>
             <c:numRef>
               <c:f>Sheet2!$D$27:$D$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>53.571428571428569</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.571428571428569</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.571428571428569</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.571428571428569</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-30.594107309425826</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9.7024715695458674</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.5829526610694693</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.9460030525478107</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.490539003586386</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
@@ -2057,10 +2088,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:legendEntry>
-        <c:idx val="6"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
@@ -2069,11 +2096,15 @@
         <c:delete val="1"/>
       </c:legendEntry>
       <c:legendEntry>
-        <c:idx val="9"/>
+        <c:idx val="11"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:legendEntry>
-        <c:idx val="10"/>
+        <c:idx val="12"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="13"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:overlay val="0"/>
@@ -4742,7 +4773,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:I26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -5908,12 +5939,12 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="P58" sqref="P58"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>